<commit_message>
added duplicates in filenames
</commit_message>
<xml_diff>
--- a/inst/extdata/CovidOISExPONTENT_CO_layout.xlsx
+++ b/inst/extdata/CovidOISExPONTENT_CO_layout.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27914"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\spelleau\OneDrive - Institut Pasteur Paris\Documents\a_Lab\z_R scripts\MFI_RAU_Gaelle_June2023\scripts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tymot\Documents\mi2lab\PvSTATEM\SerolyzeR\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88783A3D-C25C-4601-8897-3D350B706108}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2838A83-D1D4-4129-9C72-3CF05891A51E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" xr2:uid="{F9FBBE92-800C-4B3E-9D46-675E077C12B1}"/>
+    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="9960" xr2:uid="{F9FBBE92-800C-4B3E-9D46-675E077C12B1}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="100">
   <si>
     <t>A</t>
   </si>
@@ -80,12 +80,6 @@
     <t>K086-LM</t>
   </si>
   <si>
-    <t>M254-VM</t>
-  </si>
-  <si>
-    <t>M199-DS</t>
-  </si>
-  <si>
     <t>M164-LM</t>
   </si>
   <si>
@@ -312,9 +306,6 @@
   </si>
   <si>
     <t>M253-VM</t>
-  </si>
-  <si>
-    <t>M198-CN</t>
   </si>
   <si>
     <t>M163-PD</t>
@@ -351,7 +342,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -749,15 +740,15 @@
   <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15.95">
+    <row r="1" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="2">
         <v>1</v>
@@ -796,7 +787,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="15.95">
+    <row r="2" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -837,7 +828,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="15.95">
+    <row r="3" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -845,283 +836,283 @@
         <v>13</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="F3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="G3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="H3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="I3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="J3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="K3" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="L3" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="K3" s="3" t="s">
+      <c r="M3" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="L3" s="3" t="s">
+    </row>
+    <row r="4" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="M3" s="3" t="s">
+      <c r="B4" s="3" t="s">
         <v>24</v>
       </c>
+      <c r="C4" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="4" spans="1:13" ht="15.95">
-      <c r="A4" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="L4" s="3" t="s">
+    <row r="5" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="M4" s="3" t="s">
+      <c r="B5" s="3" t="s">
         <v>37</v>
       </c>
+      <c r="C5" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>48</v>
+      </c>
     </row>
-    <row r="5" spans="1:13" ht="15.95">
-      <c r="A5" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="J5" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="K5" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="L5" s="3" t="s">
+    <row r="6" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="M5" s="3" t="s">
+      <c r="B6" s="3" t="s">
         <v>50</v>
       </c>
+      <c r="C6" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="M6" s="3" t="s">
+        <v>61</v>
+      </c>
     </row>
-    <row r="6" spans="1:13" ht="15.95">
-      <c r="A6" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="J6" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="K6" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="L6" s="3" t="s">
+    <row r="7" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="M6" s="3" t="s">
+      <c r="B7" s="3" t="s">
         <v>63</v>
       </c>
+      <c r="C7" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="M7" s="3" t="s">
+        <v>74</v>
+      </c>
     </row>
-    <row r="7" spans="1:13" ht="15.95">
-      <c r="A7" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="J7" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="K7" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="L7" s="3" t="s">
+    <row r="8" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="M7" s="3" t="s">
+      <c r="B8" s="3" t="s">
         <v>76</v>
       </c>
+      <c r="C8" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="L8" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="M8" s="3" t="s">
+        <v>87</v>
+      </c>
     </row>
-    <row r="8" spans="1:13" ht="15.95">
-      <c r="A8" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="I8" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="J8" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="K8" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="L8" s="3" t="s">
+    <row r="9" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="M8" s="3" t="s">
+      <c r="B9" s="3" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" ht="15.95">
-      <c r="A9" s="1" t="s">
+      <c r="C9" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="E9" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="F9" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="G9" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="H9" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="I9" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="G9" s="3" t="s">
+      <c r="J9" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="H9" s="3" t="s">
+      <c r="K9" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="I9" s="3" t="s">
+      <c r="L9" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="J9" s="3" t="s">
+      <c r="M9" s="3" t="s">
         <v>99</v>
-      </c>
-      <c r="K9" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="L9" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="M9" s="3" t="s">
-        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added new file with duplicated names
</commit_message>
<xml_diff>
--- a/inst/extdata/CovidOISExPONTENT_CO_layout.xlsx
+++ b/inst/extdata/CovidOISExPONTENT_CO_layout.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tymot\Documents\mi2lab\PvSTATEM\SerolyzeR\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2838A83-D1D4-4129-9C72-3CF05891A51E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E36202FF-F049-442A-9900-4293F0235B00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="9960" xr2:uid="{F9FBBE92-800C-4B3E-9D46-675E077C12B1}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="103">
   <si>
     <t>A</t>
   </si>
@@ -80,6 +80,12 @@
     <t>K086-LM</t>
   </si>
   <si>
+    <t>M254-VM</t>
+  </si>
+  <si>
+    <t>M199-DS</t>
+  </si>
+  <si>
     <t>M164-LM</t>
   </si>
   <si>
@@ -306,6 +312,9 @@
   </si>
   <si>
     <t>M253-VM</t>
+  </si>
+  <si>
+    <t>M198-CN</t>
   </si>
   <si>
     <t>M163-PD</t>
@@ -740,7 +749,7 @@
   <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -836,283 +845,283 @@
         <v>13</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="L5" s="3" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="M5" s="3" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="L7" s="3" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="M7" s="3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="L8" s="3" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="M8" s="3" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>24</v>
+        <v>92</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="L9" s="3" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="M9" s="3" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: duplicates in sample names (#316)
* added duplicates in filenames

* added new file with duplicated names

* added fix

* tests and docs

* fixed sample type recognition

* updated tests

* tests update

Copilot is smart

Co-authored-by: Copilot <175728472+Copilot@users.noreply.github.com>

---------

Co-authored-by: Tymoteusz Kwiecinski <tymoteuszkwiecinski@gmail.com>
Co-authored-by: Copilot <175728472+Copilot@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/inst/extdata/CovidOISExPONTENT_CO_layout.xlsx
+++ b/inst/extdata/CovidOISExPONTENT_CO_layout.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27914"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\spelleau\OneDrive - Institut Pasteur Paris\Documents\a_Lab\z_R scripts\MFI_RAU_Gaelle_June2023\scripts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tymot\Documents\mi2lab\PvSTATEM\SerolyzeR\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88783A3D-C25C-4601-8897-3D350B706108}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E36202FF-F049-442A-9900-4293F0235B00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" xr2:uid="{F9FBBE92-800C-4B3E-9D46-675E077C12B1}"/>
+    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="9960" xr2:uid="{F9FBBE92-800C-4B3E-9D46-675E077C12B1}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -351,7 +351,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -749,15 +749,15 @@
   <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15.95">
+    <row r="1" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="2">
         <v>1</v>
@@ -796,7 +796,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="15.95">
+    <row r="2" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -837,7 +837,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="15.95">
+    <row r="3" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -878,7 +878,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="15.95">
+    <row r="4" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>25</v>
       </c>
@@ -919,7 +919,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="15.95">
+    <row r="5" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>38</v>
       </c>
@@ -960,7 +960,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="15.95">
+    <row r="6" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>51</v>
       </c>
@@ -1001,7 +1001,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="15.95">
+    <row r="7" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>64</v>
       </c>
@@ -1042,7 +1042,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="15.95">
+    <row r="8" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>77</v>
       </c>
@@ -1083,7 +1083,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="15.95">
+    <row r="9" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>90</v>
       </c>

</xml_diff>